<commit_message>
Sei lá o q mudou
</commit_message>
<xml_diff>
--- a/Pibic_pt2/SN_m_tot.xlsx
+++ b/Pibic_pt2/SN_m_tot.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Morgan-PC\Documents\pibic\Pibic_pt2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unbbr-my.sharepoint.com/personal/180075845_aluno_unb_br/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDEC2E8-712E-4C88-A4E1-382BDEC8CB6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C607C93C-4F34-4956-9B73-C994D1A4D8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -365,7 +365,7 @@
   <dimension ref="A1:D3280"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>